<commit_message>
Code fixed itself just because I looked at it? Added some preventative measures that might have been the issue but it seems more likely some dark forces are at work.
</commit_message>
<xml_diff>
--- a/app/Export/ClubAnalysisCurrent.xlsx
+++ b/app/Export/ClubAnalysisCurrent.xlsx
@@ -1991,7 +1991,7 @@
         <v>3</v>
       </c>
       <c r="AV33" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
@@ -5414,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="AV108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -6291,6 +6291,9 @@
       <c r="H124" t="n">
         <v>46.7827970091937</v>
       </c>
+      <c r="AV124" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -7101,7 +7104,7 @@
         <v>4</v>
       </c>
       <c r="AV143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -8421,6 +8424,9 @@
       <c r="H172" t="n">
         <v>38.04586400458052</v>
       </c>
+      <c r="AV172" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -14311,6 +14317,9 @@
       <c r="AM294" t="n">
         <v>1</v>
       </c>
+      <c r="AV294" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -14581,6 +14590,9 @@
       <c r="H300" t="n">
         <v>28.45213529866529</v>
       </c>
+      <c r="AV300" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -15673,6 +15685,9 @@
       <c r="H327" t="n">
         <v>53.22371484489693</v>
       </c>
+      <c r="AV327" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
@@ -16635,6 +16650,9 @@
       <c r="H349" t="n">
         <v>13.8644652312427</v>
       </c>
+      <c r="AV349" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
@@ -16828,6 +16846,9 @@
       <c r="AQ354" t="n">
         <v>1</v>
       </c>
+      <c r="AV354" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
@@ -18702,6 +18723,9 @@
       <c r="H394" t="n">
         <v>78.46207858349023</v>
       </c>
+      <c r="AV394" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
@@ -25223,6 +25247,9 @@
       <c r="H536" t="n">
         <v>77.37764416721159</v>
       </c>
+      <c r="AV536" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="537">
       <c r="A537" t="n">
@@ -26839,6 +26866,9 @@
       <c r="H570" t="n">
         <v>59.28378739710162</v>
       </c>
+      <c r="AV570" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
@@ -34170,6 +34200,9 @@
       <c r="H733" t="n">
         <v>41.51305047770984</v>
       </c>
+      <c r="AV733" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="734">
       <c r="A734" t="n">
@@ -36010,6 +36043,9 @@
       <c r="H774" t="n">
         <v>40.27709728584188</v>
       </c>
+      <c r="AV774" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="775">
       <c r="A775" t="n">
@@ -37149,6 +37185,9 @@
       </c>
       <c r="H804" t="n">
         <v>46.7964011462827</v>
+      </c>
+      <c r="AV804" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="805">

</xml_diff>